<commit_message>
Tests with different channels
</commit_message>
<xml_diff>
--- a/test_ergebnisse.xlsx
+++ b/test_ergebnisse.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2136" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="3084" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
   <si>
     <t>Feature</t>
   </si>
@@ -185,6 +185,42 @@
   </si>
   <si>
     <t>0.481</t>
+  </si>
+  <si>
+    <t>13x downsampled, 1000 datapoints</t>
+  </si>
+  <si>
+    <t>78.83</t>
+  </si>
+  <si>
+    <t>0.555</t>
+  </si>
+  <si>
+    <t>raw filtered time series</t>
+  </si>
+  <si>
+    <t>0.480</t>
+  </si>
+  <si>
+    <t>channel 46, 0.1-40</t>
+  </si>
+  <si>
+    <t>0.537</t>
+  </si>
+  <si>
+    <t>channel 40, 0.1-40</t>
+  </si>
+  <si>
+    <t>0.560</t>
+  </si>
+  <si>
+    <t>0.548</t>
+  </si>
+  <si>
+    <t>channel 40</t>
+  </si>
+  <si>
+    <t>0.873</t>
   </si>
 </sst>
 </file>
@@ -235,11 +271,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -544,15 +583,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:O27"/>
+  <dimension ref="B3:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
     <col min="3" max="3" width="18.21875" customWidth="1"/>
     <col min="4" max="4" width="8.21875" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
@@ -699,44 +738,57 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="J11" t="s">
+      <c r="C11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1711</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" t="s">
         <v>10</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="K12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="K13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
@@ -747,21 +799,18 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="K14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" t="s">
-        <v>37</v>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="K15" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
@@ -769,22 +818,28 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1147</v>
+        <v>19</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="G16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1147</v>
+      </c>
+      <c r="G17" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
@@ -795,37 +850,31 @@
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" s="1" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="N20" t="s">
-        <v>3</v>
-      </c>
-      <c r="O20" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
@@ -835,78 +884,84 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="I21" t="s">
+      <c r="N21" t="s">
+        <v>3</v>
+      </c>
+      <c r="O21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="I22" t="s">
         <v>49</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J22" t="s">
         <v>50</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N22" s="3">
         <v>7505</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O22" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J23" t="s">
         <v>52</v>
       </c>
-      <c r="N22" s="3">
+      <c r="N23" s="3">
         <v>4756</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O23" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="2">
-        <v>1344</v>
-      </c>
-      <c r="G23" t="s">
-        <v>48</v>
-      </c>
-      <c r="J23" t="s">
-        <v>55</v>
-      </c>
-      <c r="N23" s="3">
-        <v>42272</v>
-      </c>
-      <c r="O23" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1344</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J24" t="s">
+        <v>55</v>
+      </c>
+      <c r="N24" s="3">
+        <v>42272</v>
+      </c>
+      <c r="O24" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
@@ -915,6 +970,12 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
+      <c r="J25" t="s">
+        <v>57</v>
+      </c>
+      <c r="N25" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
@@ -925,12 +986,234 @@
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1735</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1807</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1799</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="2">
+        <v>3605</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1822</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>